<commit_message>
finish excel creation for register sportsman
</commit_message>
<xml_diff>
--- a/server/רישום ספורטאים למערכת.xlsx
+++ b/server/רישום ספורטאים למערכת.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ת.ז ספורטאי</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>קונגפו-פנדה (קוד: 7)</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -171,7 +174,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="26:26">
+    <row r="2" spans="4:26">
+      <c r="D2" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="Z2" s="3" t="s">
         <v>12</v>
       </c>

</xml_diff>